<commit_message>
No toques la web y la app cambie modelos
</commit_message>
<xml_diff>
--- a/tutorConnect_Tablas.xlsx
+++ b/tutorConnect_Tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredy\Documents\UIDE\Programacion Movil\Proyecto de clase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678B5C91-CC6E-4F92-9E05-4599917E1F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A615694-CB55-410E-94DA-F126B26DD03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67EC6EF7-25DE-43CF-BA44-4C89CEEE6865}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{67EC6EF7-25DE-43CF-BA44-4C89CEEE6865}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>usuarios</t>
   </si>
@@ -366,10 +366,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -714,21 +713,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291A90E1-2BAC-4CC2-A209-B80B9459FA56}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -739,24 +738,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="G2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
       <c r="J2" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -812,14 +811,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D4" t="s">
@@ -849,17 +848,17 @@
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <v>45899</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>0.625</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -870,7 +869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -884,7 +883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -897,16 +896,16 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="O7" s="6" t="s">
+      <c r="H7" s="7"/>
+      <c r="O7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
@@ -938,7 +937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G9">
         <v>1</v>
       </c>
@@ -954,10 +953,10 @@
       <c r="K9" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>0.75</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <v>0.875</v>
       </c>
       <c r="O9">
@@ -970,22 +969,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="7"/>
+      <c r="D11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1001,12 +1000,12 @@
       <c r="G12" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1016,13 +1015,13 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="7"/>
       <c r="O13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1041,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1052,7 +1051,7 @@
       <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="8" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1076,17 +1075,17 @@
       <c r="Q14" t="s">
         <v>40</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="6">
         <v>45900</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="6">
         <v>45900</v>
       </c>
       <c r="T14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1096,7 +1095,7 @@
       <c r="D15">
         <v>3</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G15">
@@ -1120,13 +1119,13 @@
       <c r="Q15" t="s">
         <v>41</v>
       </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
       <c r="T15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1136,14 +1135,14 @@
       <c r="D16">
         <v>4</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="T16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1153,12 +1152,11 @@
       <c r="D17">
         <v>5</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="T17" s="9"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1168,23 +1166,23 @@
       <c r="D18">
         <v>6</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="6" t="s">
+      <c r="O19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1201,15 +1199,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="F21" s="6" t="s">
+      <c r="B21" s="7"/>
+      <c r="F21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="7"/>
       <c r="O21">
         <v>1</v>
       </c>
@@ -1223,7 +1221,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1256,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -1281,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F24">
         <v>2</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F25">
         <v>3</v>
       </c>
@@ -1303,7 +1301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F26">
         <v>4</v>
       </c>
@@ -1314,7 +1312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F27">
         <v>5</v>
       </c>
@@ -1328,7 +1326,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F28">
         <v>6</v>
       </c>
@@ -1338,12 +1336,15 @@
       <c r="H28">
         <v>5</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="O28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P28" s="8"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
       <c r="O29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1358,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="7"/>
       <c r="O30">
         <v>1</v>
       </c>
@@ -1371,7 +1376,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O31">
         <v>2</v>
       </c>
@@ -1385,7 +1402,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
       <c r="O32">
         <v>3</v>
       </c>
@@ -1399,7 +1428,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="15:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="15:18" x14ac:dyDescent="0.3">
       <c r="O33">
         <v>4</v>
       </c>
@@ -1430,7 +1459,7 @@
       <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>